<commit_message>
Updated stories for initial quad solve
</commit_message>
<xml_diff>
--- a/Stories.xlsx
+++ b/Stories.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\GitHub\quadratic-solver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nate\Documents\GitHub\quadratic-solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Time Est.</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>Release 1</t>
+  </si>
+  <si>
+    <t>Team will put together lists of standards for the program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +107,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -192,11 +201,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -221,8 +267,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,25 +565,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="12.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -540,23 +601,22 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
@@ -568,9 +628,9 @@
       <c r="E3" s="6"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
@@ -582,37 +642,37 @@
       <c r="E4" s="6"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6">
         <v>4</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>4</v>
@@ -624,54 +684,54 @@
       <c r="E7" s="6"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="C11" s="3">
         <v>3</v>
@@ -680,54 +740,68 @@
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>